<commit_message>
fixed finale, all timings are extremely close, added 'little softer/louder' timings to ending
</commit_message>
<xml_diff>
--- a/lyrics_n_timings.xlsx
+++ b/lyrics_n_timings.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/momalave/Documents/my_virtual_envs/tiki_bird/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/momalave/Documents/my_virtual_envs/tiki_bird/tiki_room/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C121A8B-8826-E24F-B93D-E695C28AB886}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E42C7AC9-064A-0345-89CB-EA8CCC180357}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18800" yWindow="460" windowWidth="10000" windowHeight="16460" xr2:uid="{1784EFD4-1303-8844-BCCC-7FB28BBAA406}"/>
+    <workbookView xWindow="17280" yWindow="460" windowWidth="11520" windowHeight="16460" xr2:uid="{1784EFD4-1303-8844-BCCC-7FB28BBAA406}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="62">
   <si>
     <t>Enchanted Tiki Room Lyrics and Timings</t>
   </si>
@@ -272,6 +272,12 @@
   </si>
   <si>
     <t>finale</t>
+  </si>
+  <si>
+    <t>aahaa! Applause, applause</t>
+  </si>
+  <si>
+    <t>[Michael]</t>
   </si>
 </sst>
 </file>
@@ -684,10 +690,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{335B6973-0FF1-2C4F-8042-CB326E205C33}">
-  <dimension ref="A1:G145"/>
+  <dimension ref="A1:G147"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" topLeftCell="A118" workbookViewId="0">
+      <selection activeCell="A141" sqref="A141"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -1471,6 +1477,13 @@
       </c>
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A129" s="1">
+        <f>B129-B128</f>
+        <v>0.59999999999999432</v>
+      </c>
+      <c r="B129" s="1">
+        <v>191.5</v>
+      </c>
       <c r="C129" s="2" t="s">
         <v>41</v>
       </c>
@@ -1481,11 +1494,25 @@
       </c>
     </row>
     <row r="131" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A131" s="1">
+        <f>B131-B129</f>
+        <v>4.75</v>
+      </c>
+      <c r="B131" s="1">
+        <v>196.25</v>
+      </c>
       <c r="C131" s="2" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A132" s="1">
+        <f>B132-B131</f>
+        <v>1.0500000000000114</v>
+      </c>
+      <c r="B132" s="1">
+        <v>197.3</v>
+      </c>
       <c r="C132" s="2" t="s">
         <v>43</v>
       </c>
@@ -1512,11 +1539,11 @@
     </row>
     <row r="137" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A137" s="1">
-        <f>A138-B137</f>
-        <v>24.299999999999976</v>
+        <f>B137-B132</f>
+        <v>9.7999999999999829</v>
       </c>
       <c r="B137" s="1">
-        <v>1.6</v>
+        <v>207.1</v>
       </c>
       <c r="C137" s="1" t="s">
         <v>59</v>
@@ -1524,75 +1551,92 @@
     </row>
     <row r="138" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A138" s="1">
-        <f>B138-B126</f>
-        <v>25.899999999999977</v>
+        <f>B138-B137</f>
+        <v>1.8000000000000114</v>
       </c>
       <c r="B138" s="1">
+        <v>208.9</v>
+      </c>
+      <c r="C138" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="139" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C139" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="140" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A140" s="1">
+        <f>B140-B138</f>
+        <v>2.7999999999999829</v>
+      </c>
+      <c r="B140" s="1">
         <v>211.7</v>
       </c>
-      <c r="C138" s="3" t="s">
+      <c r="C140" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="G138" s="1">
+      <c r="G140" s="1">
         <v>25.9</v>
       </c>
     </row>
-    <row r="139" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C139" s="3" t="s">
+    <row r="141" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C141" s="3" t="s">
         <v>55</v>
-      </c>
-      <c r="G139" s="1">
-        <v>5.0999999999999996</v>
-      </c>
-    </row>
-    <row r="140" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G140" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="141" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A141" s="1">
-        <f>B141-B138</f>
-        <v>1.5</v>
-      </c>
-      <c r="B141" s="1">
-        <v>213.2</v>
-      </c>
-      <c r="C141" s="3" t="s">
-        <v>49</v>
       </c>
       <c r="G141" s="1">
         <v>5.0999999999999996</v>
       </c>
     </row>
     <row r="142" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C142" s="3" t="s">
-        <v>54</v>
-      </c>
       <c r="G142" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="143" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A143" s="1">
+        <f>B143-B140</f>
+        <v>1.5</v>
+      </c>
+      <c r="B143" s="1">
+        <v>213.2</v>
+      </c>
+      <c r="C143" s="3" t="s">
+        <v>49</v>
+      </c>
       <c r="G143" s="1">
-        <f>G138-(G139+G140+G141+G142)</f>
+        <v>5.0999999999999996</v>
+      </c>
+    </row>
+    <row r="144" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C144" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="G144" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="145" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G145" s="1">
+        <f>G140-(G141+G142+G143+G144)</f>
         <v>13.7</v>
       </c>
     </row>
-    <row r="144" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A144" s="1">
-        <f>B144-B141</f>
+    <row r="146" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A146" s="1">
+        <f>B146-B143</f>
         <v>3.9000000000000057</v>
       </c>
-      <c r="B144" s="1">
+      <c r="B146" s="1">
         <v>217.1</v>
       </c>
-      <c r="C144" s="3" t="s">
+      <c r="C146" s="3" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="145" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C145" s="3" t="s">
+    <row r="147" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C147" s="3" t="s">
         <v>56</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated audio file to reduce noise, simplified alltogether fnc to run faster
</commit_message>
<xml_diff>
--- a/lyrics_n_timings.xlsx
+++ b/lyrics_n_timings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/momalave/Documents/my_virtual_envs/tiki_bird/tiki_room/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E42C7AC9-064A-0345-89CB-EA8CCC180357}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C63E4BB4-4BC4-FA4C-ABAA-A0B4CE3E2FE3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17280" yWindow="460" windowWidth="11520" windowHeight="16460" xr2:uid="{1784EFD4-1303-8844-BCCC-7FB28BBAA406}"/>
+    <workbookView xWindow="9460" yWindow="460" windowWidth="19340" windowHeight="16460" xr2:uid="{1784EFD4-1303-8844-BCCC-7FB28BBAA406}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="63">
   <si>
     <t>Enchanted Tiki Room Lyrics and Timings</t>
   </si>
@@ -278,6 +278,9 @@
   </si>
   <si>
     <t>[Michael]</t>
+  </si>
+  <si>
+    <t>bam</t>
   </si>
 </sst>
 </file>
@@ -690,10 +693,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{335B6973-0FF1-2C4F-8042-CB326E205C33}">
-  <dimension ref="A1:G147"/>
+  <dimension ref="A1:G156"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A118" workbookViewId="0">
-      <selection activeCell="A141" sqref="A141"/>
+    <sheetView tabSelected="1" topLeftCell="A133" workbookViewId="0">
+      <selection activeCell="C74" sqref="C74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -1476,7 +1479,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" s="1">
         <f>B129-B128</f>
         <v>0.59999999999999432</v>
@@ -1488,12 +1491,12 @@
         <v>41</v>
       </c>
     </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C130" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" s="1">
         <f>B131-B129</f>
         <v>4.75</v>
@@ -1505,7 +1508,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="132" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" s="1">
         <f>B132-B131</f>
         <v>1.0500000000000114</v>
@@ -1517,27 +1520,27 @@
         <v>43</v>
       </c>
     </row>
-    <row r="133" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C133" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="134" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C134" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="135" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C135" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="136" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C136" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="137" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137" s="1">
         <f>B137-B132</f>
         <v>9.7999999999999829</v>
@@ -1549,94 +1552,132 @@
         <v>59</v>
       </c>
     </row>
-    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A138" s="1">
-        <f>B138-B137</f>
-        <v>1.8000000000000114</v>
-      </c>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B138" s="1">
+        <f>C138-B137</f>
+        <v>0.24000000000000909</v>
+      </c>
+      <c r="C138" s="1">
+        <v>207.34</v>
+      </c>
+      <c r="D138" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B139" s="1">
+        <f>C139-C138</f>
+        <v>0.31999999999999318</v>
+      </c>
+      <c r="C139" s="1">
+        <v>207.66</v>
+      </c>
+      <c r="D139" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B140" s="1">
+        <f>C140-C139</f>
+        <v>0.31000000000000227</v>
+      </c>
+      <c r="C140" s="1">
+        <v>207.97</v>
+      </c>
+      <c r="D140" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="146" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B146" s="1">
+        <f>B147-C140</f>
+        <v>0.93000000000000682</v>
+      </c>
+    </row>
+    <row r="147" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B147" s="1">
         <v>208.9</v>
       </c>
-      <c r="C138" s="1" t="s">
+      <c r="C147" s="1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="139" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C139" s="1" t="s">
+    <row r="148" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C148" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="140" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A140" s="1">
-        <f>B140-B138</f>
+    <row r="149" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A149" s="1">
+        <f>B149-B147</f>
         <v>2.7999999999999829</v>
       </c>
-      <c r="B140" s="1">
+      <c r="B149" s="1">
         <v>211.7</v>
       </c>
-      <c r="C140" s="3" t="s">
+      <c r="C149" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="G140" s="1">
+      <c r="G149" s="1">
         <v>25.9</v>
       </c>
     </row>
-    <row r="141" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C141" s="3" t="s">
+    <row r="150" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C150" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="G141" s="1">
+      <c r="G150" s="1">
         <v>5.0999999999999996</v>
       </c>
     </row>
-    <row r="142" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G142" s="1">
+    <row r="151" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G151" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="143" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A143" s="1">
-        <f>B143-B140</f>
+    <row r="152" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A152" s="1">
+        <f>B152-B149</f>
         <v>1.5</v>
       </c>
-      <c r="B143" s="1">
+      <c r="B152" s="1">
         <v>213.2</v>
       </c>
-      <c r="C143" s="3" t="s">
+      <c r="C152" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="G143" s="1">
+      <c r="G152" s="1">
         <v>5.0999999999999996</v>
       </c>
     </row>
-    <row r="144" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C144" s="3" t="s">
+    <row r="153" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C153" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="G144" s="1">
+      <c r="G153" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="145" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G145" s="1">
-        <f>G140-(G141+G142+G143+G144)</f>
+    <row r="154" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G154" s="1">
+        <f>G149-(G150+G151+G152+G153)</f>
         <v>13.7</v>
       </c>
     </row>
-    <row r="146" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A146" s="1">
-        <f>B146-B143</f>
+    <row r="155" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A155" s="1">
+        <f>B155-B152</f>
         <v>3.9000000000000057</v>
       </c>
-      <c r="B146" s="1">
+      <c r="B155" s="1">
         <v>217.1</v>
       </c>
-      <c r="C146" s="3" t="s">
+      <c r="C155" s="3" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="147" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C147" s="3" t="s">
+    <row r="156" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C156" s="3" t="s">
         <v>56</v>
       </c>
     </row>

</xml_diff>